<commit_message>
Common: So, liquid creation is backed by transactions from pricelist
</commit_message>
<xml_diff>
--- a/fixtures/00 - tariffs.xlsx
+++ b/fixtures/00 - tariffs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD6D9C1-2567-433F-B966-B3F64E08738C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D20A09AB-808B-4F04-98EC-70871525FF65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13965" yWindow="2025" windowWidth="23610" windowHeight="18390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4215" yWindow="2745" windowWidth="23610" windowHeight="18390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>tab</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>JX-BMD9-GYJXO9</t>
+  </si>
+  <si>
+    <t>JX-BMD9-GYJXO7</t>
   </si>
 </sst>
 </file>
@@ -459,10 +462,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27C36761-E560-4615-98DB-D2A406A4AE09}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,6 +505,17 @@
         <v>11</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Common: Welcome gifts are taken from pricelist
</commit_message>
<xml_diff>
--- a/fixtures/00 - tariffs.xlsx
+++ b/fixtures/00 - tariffs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D20A09AB-808B-4F04-98EC-70871525FF65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F8011C-E76C-492C-B237-ED3E22E68614}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4215" yWindow="2745" windowWidth="23610" windowHeight="18390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="2325" windowWidth="23610" windowHeight="18390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>tab</t>
   </si>
@@ -71,9 +71,6 @@
   </si>
   <si>
     <t>JX-BMD9-GYJXO9</t>
-  </si>
-  <si>
-    <t>JX-BMD9-GYJXO7</t>
   </si>
 </sst>
 </file>
@@ -462,10 +459,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27C36761-E560-4615-98DB-D2A406A4AE09}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,17 +502,6 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>